<commit_message>
gif for the contacts in docs
</commit_message>
<xml_diff>
--- a/Contacts.xlsx
+++ b/Contacts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -40,13 +40,31 @@
     <t>personemail@gmail.com</t>
   </si>
   <si>
-    <t>+1 9087098</t>
-  </si>
-  <si>
-    <t>Your contact person</t>
+    <t>Third Person</t>
+  </si>
+  <si>
+    <t>email@gmail.com</t>
+  </si>
+  <si>
+    <t>+91 202934880</t>
+  </si>
+  <si>
+    <t>Forth Person</t>
   </si>
   <si>
     <t>hisemail@gmail.com</t>
+  </si>
+  <si>
+    <t>+91 238907 234</t>
+  </si>
+  <si>
+    <t>Fifth person</t>
+  </si>
+  <si>
+    <t>heremail@gmail.com</t>
+  </si>
+  <si>
+    <t>+1 238974293</t>
   </si>
 </sst>
 </file>
@@ -422,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,16 +486,39 @@
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -485,8 +526,10 @@
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>